<commit_message>
Import Nilai SMK + View Nilai
</commit_message>
<xml_diff>
--- a/template_file/import_nilai_sma_ipa.xlsx
+++ b/template_file/import_nilai_sma_ipa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\sim-kcd9\template_file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B7E50E0-0134-4AB2-8F9B-7561B1B15339}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D66B20B2-3D98-4491-9C63-681C9DDED41E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AAEBBB56-5610-4DF3-8BB1-3C0F32D95CC6}"/>
   </bookViews>
@@ -99,9 +99,6 @@
     <t>LINTAS MINAT 2</t>
   </si>
   <si>
-    <t>Import Nilai</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
@@ -115,6 +112,9 @@
   </si>
   <si>
     <t>E</t>
+  </si>
+  <si>
+    <t>Import Nilai SMA IPA</t>
   </si>
 </sst>
 </file>
@@ -528,7 +528,7 @@
   <dimension ref="A1:S7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -541,7 +541,7 @@
   <sheetData>
     <row r="1" spans="1:19" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B1" s="2"/>
     </row>
@@ -609,7 +609,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>3</v>
@@ -668,7 +668,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>4</v>
@@ -727,7 +727,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>5</v>
@@ -786,7 +786,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>6</v>
@@ -845,7 +845,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>7</v>

</xml_diff>